<commit_message>
Update coding review details
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EusebiuDam\Desktop\Faculta Anul 3\Anul3Sem2\VVSS\ProiectEchipa\VVSS-Inventory-GlitchHunters\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5036CE14-DE56-4450-8589-8BD2D934E36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE09A943-4136-400D-A86B-66611D1D06E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="30240" windowHeight="17790" tabRatio="650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="30240" windowHeight="17790" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="145">
   <si>
     <t>do not print this form</t>
   </si>
@@ -242,10 +242,13 @@
     <t>Tool used:</t>
   </si>
   <si>
+    <t>SonarLint</t>
+  </si>
+  <si>
     <t>David Simonel Olimpiu</t>
   </si>
   <si>
-    <t xml:space="preserve">Mihai </t>
+    <t>15/03/2024</t>
   </si>
   <si>
     <t>File, Line</t>
@@ -1706,7 +1709,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -2075,8 +2078,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -2470,7 +2473,7 @@
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -2607,8 +2610,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="128" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView zoomScale="128" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -2682,7 +2685,9 @@
       <c r="C4" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="28"/>
+      <c r="D4" s="28" t="s">
+        <v>67</v>
+      </c>
       <c r="E4" s="28"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -2690,7 +2695,7 @@
         <v>9</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J4" s="16">
         <v>232</v>
@@ -2702,7 +2707,9 @@
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="19"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2710,9 +2717,11 @@
         <v>12</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="J5" s="16">
+        <v>232</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17"/>
@@ -2720,7 +2729,9 @@
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>69</v>
+      </c>
       <c r="E6" s="19"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -2734,16 +2745,16 @@
         <v>16</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -2756,16 +2767,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -2779,16 +2790,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -2802,16 +2813,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -2825,16 +2836,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -2848,16 +2859,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -2871,16 +2882,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
@@ -2894,16 +2905,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -2917,16 +2928,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -2940,16 +2951,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
@@ -2963,16 +2974,16 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
@@ -2986,16 +2997,16 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -3009,16 +3020,16 @@
         <v>12</v>
       </c>
       <c r="C21" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="34" t="s">
         <v>117</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>116</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
@@ -3032,16 +3043,16 @@
         <v>13</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -3055,16 +3066,16 @@
         <v>14</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
@@ -3078,16 +3089,16 @@
         <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
@@ -3101,16 +3112,16 @@
         <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17"/>
@@ -3124,16 +3135,16 @@
         <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -3147,16 +3158,16 @@
         <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
@@ -3170,16 +3181,16 @@
         <v>19</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
@@ -3202,7 +3213,7 @@
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="36" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D30" s="37"/>
       <c r="E30" s="35">

</xml_diff>